<commit_message>
sagarrokade: hlookup and documentadd for v and h lookup
</commit_message>
<xml_diff>
--- a/day-12.xlsx
+++ b/day-12.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\da24\Excel\day-12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB252EE0-FF01-4EB2-9011-A1C8BA1AC758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E5A011-16BA-49DF-9DF9-8FE88A361C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="basic" sheetId="2" r:id="rId1"/>
     <sheet name="Vlookup" sheetId="14" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="15" r:id="rId3"/>
+    <sheet name="hLookup" sheetId="15" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -939,10 +939,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F197C44-15C5-433D-A8E8-68C35A9F92B9}">
-  <dimension ref="D6:J17"/>
+  <dimension ref="C6:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" zoomScale="186" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="C6" zoomScale="176" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="E10:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -951,7 +951,7 @@
     <col min="10" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
       <c r="D6" s="6" t="s">
         <v>31</v>
       </c>
@@ -974,18 +974,36 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
       <c r="D7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-    </row>
-    <row r="8" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="E7" s="7" t="str">
+        <f>HLOOKUP(E6,$D$15:$J$17,2,FALSE)</f>
+        <v>automotive sq, near tp road , 400001</v>
+      </c>
+      <c r="F7" s="7" t="str">
+        <f t="shared" ref="F7:J7" si="0">HLOOKUP(F6,$D$15:$J$17,2,FALSE)</f>
+        <v>offline</v>
+      </c>
+      <c r="G7" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H7" s="7">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+      <c r="I7" s="7">
+        <f t="shared" si="0"/>
+        <v>100000</v>
+      </c>
+      <c r="J7" s="7">
+        <f>HLOOKUP(J6,$D$15:$J$17,2,FALSE)</f>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
       <c r="D8" s="7" t="s">
         <v>26</v>
       </c>
@@ -1008,7 +1026,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
       <c r="D9" s="7" t="s">
         <v>27</v>
       </c>
@@ -1031,18 +1049,36 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
       <c r="D10" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-    </row>
-    <row r="11" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="E10" s="7" t="str">
+        <f t="shared" ref="E10:F10" si="1">HLOOKUP(E6,$D$15:$J$17,3,FALSE)</f>
+        <v>nandanvan</v>
+      </c>
+      <c r="F10" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>online</v>
+      </c>
+      <c r="G10" s="7">
+        <f>HLOOKUP(G6,$D$15:$J$17,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H10" s="7">
+        <f t="shared" ref="H10:J10" si="2">HLOOKUP(H6,$D$15:$J$17,3,FALSE)</f>
+        <v>15000</v>
+      </c>
+      <c r="I10" s="7">
+        <f t="shared" si="2"/>
+        <v>200000</v>
+      </c>
+      <c r="J10" s="7">
+        <f t="shared" si="2"/>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
       <c r="D11" s="7" t="s">
         <v>29</v>
       </c>
@@ -1065,7 +1101,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="12" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
       <c r="D12" s="7" t="s">
         <v>30</v>
       </c>
@@ -1088,7 +1124,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>1</v>
+      </c>
       <c r="D15" s="6" t="s">
         <v>31</v>
       </c>
@@ -1111,7 +1150,10 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>2</v>
+      </c>
       <c r="D16" s="7" t="s">
         <v>25</v>
       </c>
@@ -1134,7 +1176,10 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="17" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>3</v>
+      </c>
       <c r="D17" s="7" t="s">
         <v>28</v>
       </c>

</xml_diff>